<commit_message>
New layout and warps (but the AI is got broken)
</commit_message>
<xml_diff>
--- a/ScreenMap.xlsx
+++ b/ScreenMap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcerdeira\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcerdeira\beel\Test\Lolo\Lolo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>00</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>15</t>
+  </si>
+  <si>
+    <t>Fixed Empty</t>
+  </si>
+  <si>
+    <t>Fixed Unbreakable</t>
+  </si>
+  <si>
+    <t>Warp Zone</t>
+  </si>
+  <si>
+    <t>Available for random</t>
   </si>
 </sst>
 </file>
@@ -87,7 +99,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,7 +120,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -125,12 +143,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,86 +442,86 @@
     <col min="1" max="17" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -510,17 +530,21 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
+      <c r="O3" s="5"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="Q3" s="5"/>
+      <c r="S3" s="1"/>
+      <c r="T3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="5"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -529,21 +553,25 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="M4" s="5"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="Q4" s="5"/>
+      <c r="S4" s="2"/>
+      <c r="T4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -552,17 +580,21 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+      <c r="O5" s="5"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="Q5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -571,21 +603,25 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+      <c r="M6" s="5"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="Q6" s="5"/>
+      <c r="S6" s="6"/>
+      <c r="T6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -594,40 +630,40 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
+      <c r="O7" s="5"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="Q7" s="6"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="5"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
+      <c r="M8" s="5"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="Q8" s="6"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -636,17 +672,17 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
+      <c r="O9" s="5"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="Q9" s="5"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -655,21 +691,21 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
+      <c r="M10" s="5"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="Q10" s="5"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -678,17 +714,17 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="O11" s="5"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="5"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -697,32 +733,33 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
+      <c r="M12" s="5"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="2"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="4"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="3"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Path finding solution started
All movement based solutions seems to suck
</commit_message>
<xml_diff>
--- a/ScreenMap.xlsx
+++ b/ScreenMap.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Basic Layout" sheetId="1" r:id="rId1"/>
+    <sheet name="Layout with X, Y" sheetId="3" r:id="rId2"/>
+    <sheet name="Layout in List" sheetId="4" r:id="rId3"/>
+    <sheet name="tmp" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="46">
   <si>
     <t>00</t>
   </si>
@@ -116,13 +117,61 @@
   </si>
   <si>
     <t>r=4</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>350</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>450</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>550</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>650</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>750</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,8 +186,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +238,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -188,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -200,6 +275,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,10 +902,1704 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="16" t="str">
+        <f>B$14 &amp; "," &amp; $R2</f>
+        <v>0,0</v>
+      </c>
+      <c r="C2" s="16" t="str">
+        <f>C$14 &amp; "," &amp; $R2</f>
+        <v>50,0</v>
+      </c>
+      <c r="D2" s="16" t="str">
+        <f t="shared" ref="D2:Q4" si="0">D$14 &amp; "," &amp; $R2</f>
+        <v>100,0</v>
+      </c>
+      <c r="E2" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>150,0</v>
+      </c>
+      <c r="F2" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>200,0</v>
+      </c>
+      <c r="G2" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>250,0</v>
+      </c>
+      <c r="H2" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>300,0</v>
+      </c>
+      <c r="I2" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>350,0</v>
+      </c>
+      <c r="J2" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>400,0</v>
+      </c>
+      <c r="K2" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>450,0</v>
+      </c>
+      <c r="L2" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>500,0</v>
+      </c>
+      <c r="M2" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>550,0</v>
+      </c>
+      <c r="N2" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>600,0</v>
+      </c>
+      <c r="O2" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>650,0</v>
+      </c>
+      <c r="P2" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>700,0</v>
+      </c>
+      <c r="Q2" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>750,0</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16" t="str">
+        <f>B$14 &amp; "," &amp; $R3</f>
+        <v>0,50</v>
+      </c>
+      <c r="C3" s="14" t="str">
+        <f>C$14 &amp; "," &amp; $R3</f>
+        <v>50,50</v>
+      </c>
+      <c r="D3" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>100,50</v>
+      </c>
+      <c r="E3" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>150,50</v>
+      </c>
+      <c r="F3" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>200,50</v>
+      </c>
+      <c r="G3" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>250,50</v>
+      </c>
+      <c r="H3" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>300,50</v>
+      </c>
+      <c r="I3" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>350,50</v>
+      </c>
+      <c r="J3" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>400,50</v>
+      </c>
+      <c r="K3" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>450,50</v>
+      </c>
+      <c r="L3" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>500,50</v>
+      </c>
+      <c r="M3" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>550,50</v>
+      </c>
+      <c r="N3" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>600,50</v>
+      </c>
+      <c r="O3" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>650,50</v>
+      </c>
+      <c r="P3" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>700,50</v>
+      </c>
+      <c r="Q3" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>750,50</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16" t="str">
+        <f>B$14 &amp; "," &amp; $R4</f>
+        <v>0,100</v>
+      </c>
+      <c r="C4" s="14" t="str">
+        <f t="shared" ref="C4:P4" si="1">C$14 &amp; "," &amp; $R4</f>
+        <v>50,100</v>
+      </c>
+      <c r="D4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>100,100</v>
+      </c>
+      <c r="E4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>150,100</v>
+      </c>
+      <c r="F4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>200,100</v>
+      </c>
+      <c r="G4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>250,100</v>
+      </c>
+      <c r="H4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>300,100</v>
+      </c>
+      <c r="I4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>350,100</v>
+      </c>
+      <c r="J4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>400,100</v>
+      </c>
+      <c r="K4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>450,100</v>
+      </c>
+      <c r="L4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>500,100</v>
+      </c>
+      <c r="M4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>550,100</v>
+      </c>
+      <c r="N4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>600,100</v>
+      </c>
+      <c r="O4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>650,100</v>
+      </c>
+      <c r="P4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>700,100</v>
+      </c>
+      <c r="Q4" s="16" t="str">
+        <f>Q$14 &amp; "," &amp; $R4</f>
+        <v>750,100</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="16" t="str">
+        <f t="shared" ref="B5:Q13" si="2">B$14 &amp; "," &amp; $R5</f>
+        <v>0,150</v>
+      </c>
+      <c r="C5" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>50,150</v>
+      </c>
+      <c r="D5" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>100,150</v>
+      </c>
+      <c r="E5" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>150,150</v>
+      </c>
+      <c r="F5" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>200,150</v>
+      </c>
+      <c r="G5" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>250,150</v>
+      </c>
+      <c r="H5" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>300,150</v>
+      </c>
+      <c r="I5" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>350,150</v>
+      </c>
+      <c r="J5" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>400,150</v>
+      </c>
+      <c r="K5" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>450,150</v>
+      </c>
+      <c r="L5" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>500,150</v>
+      </c>
+      <c r="M5" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>550,150</v>
+      </c>
+      <c r="N5" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>600,150</v>
+      </c>
+      <c r="O5" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>650,150</v>
+      </c>
+      <c r="P5" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>700,150</v>
+      </c>
+      <c r="Q5" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>750,150</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>0,200</v>
+      </c>
+      <c r="C6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>50,200</v>
+      </c>
+      <c r="D6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>100,200</v>
+      </c>
+      <c r="E6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>150,200</v>
+      </c>
+      <c r="F6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>200,200</v>
+      </c>
+      <c r="G6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>250,200</v>
+      </c>
+      <c r="H6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>300,200</v>
+      </c>
+      <c r="I6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>350,200</v>
+      </c>
+      <c r="J6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>400,200</v>
+      </c>
+      <c r="K6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>450,200</v>
+      </c>
+      <c r="L6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>500,200</v>
+      </c>
+      <c r="M6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>550,200</v>
+      </c>
+      <c r="N6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>600,200</v>
+      </c>
+      <c r="O6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>650,200</v>
+      </c>
+      <c r="P6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>700,200</v>
+      </c>
+      <c r="Q6" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>750,200</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>0,250</v>
+      </c>
+      <c r="C7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>50,250</v>
+      </c>
+      <c r="D7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>100,250</v>
+      </c>
+      <c r="E7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>150,250</v>
+      </c>
+      <c r="F7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>200,250</v>
+      </c>
+      <c r="G7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>250,250</v>
+      </c>
+      <c r="H7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>300,250</v>
+      </c>
+      <c r="I7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>350,250</v>
+      </c>
+      <c r="J7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>400,250</v>
+      </c>
+      <c r="K7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>450,250</v>
+      </c>
+      <c r="L7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>500,250</v>
+      </c>
+      <c r="M7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>550,250</v>
+      </c>
+      <c r="N7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>600,250</v>
+      </c>
+      <c r="O7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>650,250</v>
+      </c>
+      <c r="P7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>700,250</v>
+      </c>
+      <c r="Q7" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>750,250</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>0,300</v>
+      </c>
+      <c r="C8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>50,300</v>
+      </c>
+      <c r="D8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>100,300</v>
+      </c>
+      <c r="E8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>150,300</v>
+      </c>
+      <c r="F8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>200,300</v>
+      </c>
+      <c r="G8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>250,300</v>
+      </c>
+      <c r="H8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>300,300</v>
+      </c>
+      <c r="I8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>350,300</v>
+      </c>
+      <c r="J8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>400,300</v>
+      </c>
+      <c r="K8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>450,300</v>
+      </c>
+      <c r="L8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>500,300</v>
+      </c>
+      <c r="M8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>550,300</v>
+      </c>
+      <c r="N8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>600,300</v>
+      </c>
+      <c r="O8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>650,300</v>
+      </c>
+      <c r="P8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>700,300</v>
+      </c>
+      <c r="Q8" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>750,300</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>0,350</v>
+      </c>
+      <c r="C9" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>50,350</v>
+      </c>
+      <c r="D9" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>100,350</v>
+      </c>
+      <c r="E9" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>150,350</v>
+      </c>
+      <c r="F9" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>200,350</v>
+      </c>
+      <c r="G9" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>250,350</v>
+      </c>
+      <c r="H9" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>300,350</v>
+      </c>
+      <c r="I9" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>350,350</v>
+      </c>
+      <c r="J9" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>400,350</v>
+      </c>
+      <c r="K9" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>450,350</v>
+      </c>
+      <c r="L9" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>500,350</v>
+      </c>
+      <c r="M9" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>550,350</v>
+      </c>
+      <c r="N9" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>600,350</v>
+      </c>
+      <c r="O9" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>650,350</v>
+      </c>
+      <c r="P9" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>700,350</v>
+      </c>
+      <c r="Q9" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>750,350</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>0,400</v>
+      </c>
+      <c r="C10" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>50,400</v>
+      </c>
+      <c r="D10" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>100,400</v>
+      </c>
+      <c r="E10" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>150,400</v>
+      </c>
+      <c r="F10" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>200,400</v>
+      </c>
+      <c r="G10" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>250,400</v>
+      </c>
+      <c r="H10" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>300,400</v>
+      </c>
+      <c r="I10" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>350,400</v>
+      </c>
+      <c r="J10" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>400,400</v>
+      </c>
+      <c r="K10" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>450,400</v>
+      </c>
+      <c r="L10" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>500,400</v>
+      </c>
+      <c r="M10" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>550,400</v>
+      </c>
+      <c r="N10" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>600,400</v>
+      </c>
+      <c r="O10" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>650,400</v>
+      </c>
+      <c r="P10" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>700,400</v>
+      </c>
+      <c r="Q10" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>750,400</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>0,450</v>
+      </c>
+      <c r="C11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>50,450</v>
+      </c>
+      <c r="D11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>100,450</v>
+      </c>
+      <c r="E11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>150,450</v>
+      </c>
+      <c r="F11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>200,450</v>
+      </c>
+      <c r="G11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>250,450</v>
+      </c>
+      <c r="H11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>300,450</v>
+      </c>
+      <c r="I11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>350,450</v>
+      </c>
+      <c r="J11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>400,450</v>
+      </c>
+      <c r="K11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>450,450</v>
+      </c>
+      <c r="L11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>500,450</v>
+      </c>
+      <c r="M11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>550,450</v>
+      </c>
+      <c r="N11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>600,450</v>
+      </c>
+      <c r="O11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>650,450</v>
+      </c>
+      <c r="P11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>700,450</v>
+      </c>
+      <c r="Q11" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>750,450</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>0,500</v>
+      </c>
+      <c r="C12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>50,500</v>
+      </c>
+      <c r="D12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>100,500</v>
+      </c>
+      <c r="E12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>150,500</v>
+      </c>
+      <c r="F12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>200,500</v>
+      </c>
+      <c r="G12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>250,500</v>
+      </c>
+      <c r="H12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>300,500</v>
+      </c>
+      <c r="I12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>350,500</v>
+      </c>
+      <c r="J12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>400,500</v>
+      </c>
+      <c r="K12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>450,500</v>
+      </c>
+      <c r="L12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>500,500</v>
+      </c>
+      <c r="M12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>550,500</v>
+      </c>
+      <c r="N12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>600,500</v>
+      </c>
+      <c r="O12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>650,500</v>
+      </c>
+      <c r="P12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>700,500</v>
+      </c>
+      <c r="Q12" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>750,500</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>0,550</v>
+      </c>
+      <c r="C13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>50,550</v>
+      </c>
+      <c r="D13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>100,550</v>
+      </c>
+      <c r="E13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>150,550</v>
+      </c>
+      <c r="F13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>200,550</v>
+      </c>
+      <c r="G13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>250,550</v>
+      </c>
+      <c r="H13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>300,550</v>
+      </c>
+      <c r="I13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>350,550</v>
+      </c>
+      <c r="J13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>400,550</v>
+      </c>
+      <c r="K13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>450,550</v>
+      </c>
+      <c r="L13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>500,550</v>
+      </c>
+      <c r="M13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>550,550</v>
+      </c>
+      <c r="N13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>600,550</v>
+      </c>
+      <c r="O13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>650,550</v>
+      </c>
+      <c r="P13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>700,550</v>
+      </c>
+      <c r="Q13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>750,550</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="9" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="17" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13">
+        <v>1</v>
+      </c>
+      <c r="D2" s="13">
+        <v>2</v>
+      </c>
+      <c r="E2" s="13">
+        <v>3</v>
+      </c>
+      <c r="F2" s="13">
+        <v>4</v>
+      </c>
+      <c r="G2" s="13">
+        <v>5</v>
+      </c>
+      <c r="H2" s="13">
+        <v>6</v>
+      </c>
+      <c r="I2" s="13">
+        <v>7</v>
+      </c>
+      <c r="J2" s="19">
+        <v>96</v>
+      </c>
+      <c r="K2" s="19">
+        <v>97</v>
+      </c>
+      <c r="L2" s="19">
+        <v>98</v>
+      </c>
+      <c r="M2" s="19">
+        <v>99</v>
+      </c>
+      <c r="N2" s="19">
+        <v>100</v>
+      </c>
+      <c r="O2" s="19">
+        <v>101</v>
+      </c>
+      <c r="P2" s="19">
+        <v>102</v>
+      </c>
+      <c r="Q2" s="19">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14">
+        <v>9</v>
+      </c>
+      <c r="D3" s="14">
+        <v>10</v>
+      </c>
+      <c r="E3" s="14">
+        <v>11</v>
+      </c>
+      <c r="F3" s="14">
+        <v>12</v>
+      </c>
+      <c r="G3" s="14">
+        <v>13</v>
+      </c>
+      <c r="H3" s="14">
+        <v>14</v>
+      </c>
+      <c r="I3" s="14">
+        <v>15</v>
+      </c>
+      <c r="J3" s="18">
+        <v>104</v>
+      </c>
+      <c r="K3" s="18">
+        <v>105</v>
+      </c>
+      <c r="L3" s="18">
+        <v>106</v>
+      </c>
+      <c r="M3" s="18">
+        <v>107</v>
+      </c>
+      <c r="N3" s="18">
+        <v>108</v>
+      </c>
+      <c r="O3" s="18">
+        <v>109</v>
+      </c>
+      <c r="P3" s="18">
+        <v>110</v>
+      </c>
+      <c r="Q3" s="19">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13">
+        <v>16</v>
+      </c>
+      <c r="C4" s="14">
+        <v>17</v>
+      </c>
+      <c r="D4" s="14">
+        <v>18</v>
+      </c>
+      <c r="E4" s="14">
+        <v>19</v>
+      </c>
+      <c r="F4" s="14">
+        <v>20</v>
+      </c>
+      <c r="G4" s="14">
+        <v>21</v>
+      </c>
+      <c r="H4" s="14">
+        <v>22</v>
+      </c>
+      <c r="I4" s="14">
+        <v>23</v>
+      </c>
+      <c r="J4" s="18">
+        <v>112</v>
+      </c>
+      <c r="K4" s="18">
+        <v>113</v>
+      </c>
+      <c r="L4" s="18">
+        <v>114</v>
+      </c>
+      <c r="M4" s="18">
+        <v>115</v>
+      </c>
+      <c r="N4" s="18">
+        <v>116</v>
+      </c>
+      <c r="O4" s="18">
+        <v>117</v>
+      </c>
+      <c r="P4" s="18">
+        <v>118</v>
+      </c>
+      <c r="Q4" s="19">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="13">
+        <v>24</v>
+      </c>
+      <c r="C5" s="14">
+        <v>25</v>
+      </c>
+      <c r="D5" s="14">
+        <v>26</v>
+      </c>
+      <c r="E5" s="14">
+        <v>27</v>
+      </c>
+      <c r="F5" s="14">
+        <v>28</v>
+      </c>
+      <c r="G5" s="14">
+        <v>29</v>
+      </c>
+      <c r="H5" s="14">
+        <v>30</v>
+      </c>
+      <c r="I5" s="14">
+        <v>31</v>
+      </c>
+      <c r="J5" s="18">
+        <v>120</v>
+      </c>
+      <c r="K5" s="18">
+        <v>121</v>
+      </c>
+      <c r="L5" s="18">
+        <v>122</v>
+      </c>
+      <c r="M5" s="18">
+        <v>123</v>
+      </c>
+      <c r="N5" s="18">
+        <v>124</v>
+      </c>
+      <c r="O5" s="18">
+        <v>125</v>
+      </c>
+      <c r="P5" s="18">
+        <v>126</v>
+      </c>
+      <c r="Q5" s="19">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="13">
+        <v>32</v>
+      </c>
+      <c r="C6" s="14">
+        <v>33</v>
+      </c>
+      <c r="D6" s="14">
+        <v>34</v>
+      </c>
+      <c r="E6" s="14">
+        <v>35</v>
+      </c>
+      <c r="F6" s="14">
+        <v>36</v>
+      </c>
+      <c r="G6" s="14">
+        <v>37</v>
+      </c>
+      <c r="H6" s="14">
+        <v>38</v>
+      </c>
+      <c r="I6" s="14">
+        <v>39</v>
+      </c>
+      <c r="J6" s="18">
+        <v>128</v>
+      </c>
+      <c r="K6" s="18">
+        <v>129</v>
+      </c>
+      <c r="L6" s="18">
+        <v>130</v>
+      </c>
+      <c r="M6" s="18">
+        <v>131</v>
+      </c>
+      <c r="N6" s="18">
+        <v>132</v>
+      </c>
+      <c r="O6" s="18">
+        <v>133</v>
+      </c>
+      <c r="P6" s="18">
+        <v>134</v>
+      </c>
+      <c r="Q6" s="19">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="15">
+        <v>40</v>
+      </c>
+      <c r="C7" s="14">
+        <v>41</v>
+      </c>
+      <c r="D7" s="14">
+        <v>42</v>
+      </c>
+      <c r="E7" s="14">
+        <v>43</v>
+      </c>
+      <c r="F7" s="14">
+        <v>44</v>
+      </c>
+      <c r="G7" s="14">
+        <v>45</v>
+      </c>
+      <c r="H7" s="14">
+        <v>46</v>
+      </c>
+      <c r="I7" s="14">
+        <v>47</v>
+      </c>
+      <c r="J7" s="18">
+        <v>136</v>
+      </c>
+      <c r="K7" s="18">
+        <v>137</v>
+      </c>
+      <c r="L7" s="18">
+        <v>138</v>
+      </c>
+      <c r="M7" s="18">
+        <v>139</v>
+      </c>
+      <c r="N7" s="18">
+        <v>140</v>
+      </c>
+      <c r="O7" s="18">
+        <v>141</v>
+      </c>
+      <c r="P7" s="18">
+        <v>142</v>
+      </c>
+      <c r="Q7" s="15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="15">
+        <v>48</v>
+      </c>
+      <c r="C8" s="14">
+        <v>49</v>
+      </c>
+      <c r="D8" s="14">
+        <v>50</v>
+      </c>
+      <c r="E8" s="14">
+        <v>51</v>
+      </c>
+      <c r="F8" s="14">
+        <v>52</v>
+      </c>
+      <c r="G8" s="14">
+        <v>53</v>
+      </c>
+      <c r="H8" s="14">
+        <v>54</v>
+      </c>
+      <c r="I8" s="14">
+        <v>55</v>
+      </c>
+      <c r="J8" s="18">
+        <v>144</v>
+      </c>
+      <c r="K8" s="18">
+        <v>145</v>
+      </c>
+      <c r="L8" s="18">
+        <v>146</v>
+      </c>
+      <c r="M8" s="18">
+        <v>147</v>
+      </c>
+      <c r="N8" s="18">
+        <v>148</v>
+      </c>
+      <c r="O8" s="18">
+        <v>149</v>
+      </c>
+      <c r="P8" s="18">
+        <v>150</v>
+      </c>
+      <c r="Q8" s="15">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="13">
+        <v>56</v>
+      </c>
+      <c r="C9" s="14">
+        <v>57</v>
+      </c>
+      <c r="D9" s="14">
+        <v>58</v>
+      </c>
+      <c r="E9" s="14">
+        <v>59</v>
+      </c>
+      <c r="F9" s="14">
+        <v>60</v>
+      </c>
+      <c r="G9" s="14">
+        <v>61</v>
+      </c>
+      <c r="H9" s="14">
+        <v>62</v>
+      </c>
+      <c r="I9" s="14">
+        <v>63</v>
+      </c>
+      <c r="J9" s="18">
+        <v>152</v>
+      </c>
+      <c r="K9" s="18">
+        <v>153</v>
+      </c>
+      <c r="L9" s="18">
+        <v>154</v>
+      </c>
+      <c r="M9" s="18">
+        <v>155</v>
+      </c>
+      <c r="N9" s="18">
+        <v>156</v>
+      </c>
+      <c r="O9" s="18">
+        <v>157</v>
+      </c>
+      <c r="P9" s="18">
+        <v>158</v>
+      </c>
+      <c r="Q9" s="19">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13">
+        <v>64</v>
+      </c>
+      <c r="C10" s="14">
+        <v>65</v>
+      </c>
+      <c r="D10" s="14">
+        <v>66</v>
+      </c>
+      <c r="E10" s="14">
+        <v>67</v>
+      </c>
+      <c r="F10" s="14">
+        <v>68</v>
+      </c>
+      <c r="G10" s="14">
+        <v>69</v>
+      </c>
+      <c r="H10" s="14">
+        <v>70</v>
+      </c>
+      <c r="I10" s="14">
+        <v>71</v>
+      </c>
+      <c r="J10" s="18">
+        <v>160</v>
+      </c>
+      <c r="K10" s="18">
+        <v>161</v>
+      </c>
+      <c r="L10" s="18">
+        <v>162</v>
+      </c>
+      <c r="M10" s="18">
+        <v>163</v>
+      </c>
+      <c r="N10" s="18">
+        <v>164</v>
+      </c>
+      <c r="O10" s="18">
+        <v>165</v>
+      </c>
+      <c r="P10" s="18">
+        <v>166</v>
+      </c>
+      <c r="Q10" s="19">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="13">
+        <v>72</v>
+      </c>
+      <c r="C11" s="14">
+        <v>73</v>
+      </c>
+      <c r="D11" s="14">
+        <v>74</v>
+      </c>
+      <c r="E11" s="14">
+        <v>75</v>
+      </c>
+      <c r="F11" s="14">
+        <v>76</v>
+      </c>
+      <c r="G11" s="14">
+        <v>77</v>
+      </c>
+      <c r="H11" s="14">
+        <v>78</v>
+      </c>
+      <c r="I11" s="14">
+        <v>79</v>
+      </c>
+      <c r="J11" s="18">
+        <v>168</v>
+      </c>
+      <c r="K11" s="18">
+        <v>169</v>
+      </c>
+      <c r="L11" s="18">
+        <v>170</v>
+      </c>
+      <c r="M11" s="18">
+        <v>171</v>
+      </c>
+      <c r="N11" s="18">
+        <v>172</v>
+      </c>
+      <c r="O11" s="18">
+        <v>173</v>
+      </c>
+      <c r="P11" s="18">
+        <v>174</v>
+      </c>
+      <c r="Q11" s="19">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="13">
+        <v>80</v>
+      </c>
+      <c r="C12" s="14">
+        <v>81</v>
+      </c>
+      <c r="D12" s="14">
+        <v>82</v>
+      </c>
+      <c r="E12" s="14">
+        <v>83</v>
+      </c>
+      <c r="F12" s="14">
+        <v>84</v>
+      </c>
+      <c r="G12" s="14">
+        <v>85</v>
+      </c>
+      <c r="H12" s="14">
+        <v>86</v>
+      </c>
+      <c r="I12" s="14">
+        <v>87</v>
+      </c>
+      <c r="J12" s="18">
+        <v>176</v>
+      </c>
+      <c r="K12" s="18">
+        <v>177</v>
+      </c>
+      <c r="L12" s="18">
+        <v>178</v>
+      </c>
+      <c r="M12" s="18">
+        <v>179</v>
+      </c>
+      <c r="N12" s="18">
+        <v>180</v>
+      </c>
+      <c r="O12" s="18">
+        <v>181</v>
+      </c>
+      <c r="P12" s="18">
+        <v>182</v>
+      </c>
+      <c r="Q12" s="19">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="13">
+        <v>88</v>
+      </c>
+      <c r="C13" s="13">
+        <v>89</v>
+      </c>
+      <c r="D13" s="13">
+        <v>90</v>
+      </c>
+      <c r="E13" s="13">
+        <v>91</v>
+      </c>
+      <c r="F13" s="13">
+        <v>92</v>
+      </c>
+      <c r="G13" s="13">
+        <v>93</v>
+      </c>
+      <c r="H13" s="13">
+        <v>94</v>
+      </c>
+      <c r="I13" s="13">
+        <v>95</v>
+      </c>
+      <c r="J13" s="19">
+        <v>184</v>
+      </c>
+      <c r="K13" s="19">
+        <v>185</v>
+      </c>
+      <c r="L13" s="19">
+        <v>186</v>
+      </c>
+      <c r="M13" s="19">
+        <v>187</v>
+      </c>
+      <c r="N13" s="19">
+        <v>188</v>
+      </c>
+      <c r="O13" s="19">
+        <v>189</v>
+      </c>
+      <c r="P13" s="19">
+        <v>190</v>
+      </c>
+      <c r="Q13" s="19">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,324 +2981,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="17" width="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="5"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="5"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="5"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="5"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="6"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="6"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="5"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="5"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="5"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="5"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Starting to implement the AI, to see it and debug
</commit_message>
<xml_diff>
--- a/ScreenMap.xlsx
+++ b/ScreenMap.xlsx
@@ -202,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,12 +257,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -276,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -298,8 +292,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2612,10 +2604,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,7 +2616,7 @@
     <col min="10" max="17" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
       <c r="B1" s="12" t="s">
         <v>0</v>
@@ -2675,7 +2667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
@@ -2728,7 +2720,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
@@ -2738,10 +2730,10 @@
       <c r="C3" s="20">
         <v>9</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="20">
         <v>10</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="20">
         <v>11</v>
       </c>
       <c r="F3" s="20">
@@ -2781,7 +2773,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -2794,10 +2786,10 @@
       <c r="D4" s="20">
         <v>18</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="20">
         <v>19</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="20">
         <v>20</v>
       </c>
       <c r="G4" s="20">
@@ -2834,7 +2826,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
@@ -2887,7 +2879,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
@@ -2940,7 +2932,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
@@ -2993,7 +2985,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
@@ -3046,7 +3038,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -3099,7 +3091,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
@@ -3151,9 +3143,8 @@
       <c r="Q10" s="19">
         <v>167</v>
       </c>
-      <c r="U10" s="22"/>
-    </row>
-    <row r="11" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
@@ -3206,7 +3197,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
@@ -3259,7 +3250,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Some fixes on v0, It still kinda sucks
</commit_message>
<xml_diff>
--- a/ScreenMap.xlsx
+++ b/ScreenMap.xlsx
@@ -172,7 +172,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,8 +201,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,6 +263,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -270,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -292,6 +304,8 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -913,7 +927,7 @@
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1901,7 +1915,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:R14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2607,7 +2621,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2727,25 +2741,25 @@
       <c r="B3" s="13">
         <v>8</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="21">
         <v>9</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="21">
         <v>10</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="21">
         <v>11</v>
       </c>
       <c r="F3" s="20">
         <v>12</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="21">
         <v>13</v>
       </c>
-      <c r="H3" s="20">
+      <c r="H3" s="21">
         <v>14</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3" s="21">
         <v>15</v>
       </c>
       <c r="J3" s="20">
@@ -2754,19 +2768,19 @@
       <c r="K3" s="20">
         <v>105</v>
       </c>
-      <c r="L3" s="20">
+      <c r="L3" s="21">
         <v>106</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="21">
         <v>107</v>
       </c>
-      <c r="N3" s="20">
+      <c r="N3" s="21">
         <v>108</v>
       </c>
       <c r="O3" s="20">
         <v>109</v>
       </c>
-      <c r="P3" s="20">
+      <c r="P3" s="21">
         <v>110</v>
       </c>
       <c r="Q3" s="19">
@@ -2780,46 +2794,46 @@
       <c r="B4" s="13">
         <v>16</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="21">
         <v>17</v>
       </c>
       <c r="D4" s="20">
         <v>18</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="21">
         <v>19</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="21">
         <v>20</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="21">
         <v>21</v>
       </c>
-      <c r="H4" s="20">
+      <c r="H4" s="21">
         <v>22</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="21">
         <v>23</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="21">
         <v>112</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4" s="21">
         <v>113</v>
       </c>
-      <c r="L4" s="20">
+      <c r="L4" s="21">
         <v>114</v>
       </c>
       <c r="M4" s="20">
         <v>115</v>
       </c>
-      <c r="N4" s="20">
+      <c r="N4" s="21">
         <v>116</v>
       </c>
-      <c r="O4" s="20">
+      <c r="O4" s="21">
         <v>117</v>
       </c>
-      <c r="P4" s="20">
+      <c r="P4" s="21">
         <v>118</v>
       </c>
       <c r="Q4" s="19">
@@ -2833,10 +2847,10 @@
       <c r="B5" s="13">
         <v>24</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="21">
         <v>25</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="22">
         <v>26</v>
       </c>
       <c r="E5" s="20">
@@ -2845,34 +2859,34 @@
       <c r="F5" s="20">
         <v>28</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="21">
         <v>29</v>
       </c>
       <c r="H5" s="20">
         <v>30</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="21">
         <v>31</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="21">
         <v>120</v>
       </c>
-      <c r="K5" s="20">
+      <c r="K5" s="21">
         <v>121</v>
       </c>
-      <c r="L5" s="20">
+      <c r="L5" s="21">
         <v>122</v>
       </c>
-      <c r="M5" s="20">
+      <c r="M5" s="21">
         <v>123</v>
       </c>
-      <c r="N5" s="20">
+      <c r="N5" s="21">
         <v>124</v>
       </c>
       <c r="O5" s="20">
         <v>125</v>
       </c>
-      <c r="P5" s="20">
+      <c r="P5" s="21">
         <v>126</v>
       </c>
       <c r="Q5" s="19">
@@ -2892,19 +2906,19 @@
       <c r="D6" s="20">
         <v>34</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="21">
         <v>35</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="21">
         <v>36</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="21">
         <v>37</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="21">
         <v>38</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="21">
         <v>39</v>
       </c>
       <c r="J6" s="20">
@@ -2919,13 +2933,13 @@
       <c r="M6" s="20">
         <v>131</v>
       </c>
-      <c r="N6" s="20">
+      <c r="N6" s="21">
         <v>132</v>
       </c>
-      <c r="O6" s="20">
+      <c r="O6" s="21">
         <v>133</v>
       </c>
-      <c r="P6" s="20">
+      <c r="P6" s="21">
         <v>134</v>
       </c>
       <c r="Q6" s="19">
@@ -2945,7 +2959,7 @@
       <c r="D7" s="20">
         <v>42</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="21">
         <v>43</v>
       </c>
       <c r="F7" s="20">

</xml_diff>

<commit_message>
Some menu interactions and more Path finding
</commit_message>
<xml_diff>
--- a/ScreenMap.xlsx
+++ b/ScreenMap.xlsx
@@ -208,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,13 +265,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -312,7 +306,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2628,7 +2621,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2807,7 +2800,7 @@
       <c r="D4" s="20">
         <v>18</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="20">
         <v>19</v>
       </c>
       <c r="F4" s="20">
@@ -3084,7 +3077,7 @@
       <c r="H9" s="20">
         <v>62</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="22">
         <v>63</v>
       </c>
       <c r="J9" s="20">
@@ -3137,10 +3130,10 @@
       <c r="H10" s="20">
         <v>70</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="22">
         <v>71</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="22">
         <v>160</v>
       </c>
       <c r="K10" s="20">
@@ -3155,7 +3148,7 @@
       <c r="N10" s="20">
         <v>164</v>
       </c>
-      <c r="O10" s="23">
+      <c r="O10" s="20">
         <v>165</v>
       </c>
       <c r="P10" s="20">
@@ -3193,25 +3186,25 @@
       <c r="I11" s="20">
         <v>79</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="22">
         <v>168</v>
       </c>
-      <c r="K11" s="20">
+      <c r="K11" s="22">
         <v>169</v>
       </c>
-      <c r="L11" s="20">
+      <c r="L11" s="22">
         <v>170</v>
       </c>
-      <c r="M11" s="20">
+      <c r="M11" s="22">
         <v>171</v>
       </c>
-      <c r="N11" s="20">
+      <c r="N11" s="22">
         <v>172</v>
       </c>
       <c r="O11" s="20">
         <v>173</v>
       </c>
-      <c r="P11" s="20">
+      <c r="P11" s="22">
         <v>174</v>
       </c>
       <c r="Q11" s="19">
@@ -3258,13 +3251,13 @@
       <c r="M12" s="20">
         <v>179</v>
       </c>
-      <c r="N12" s="20">
+      <c r="N12" s="22">
         <v>180</v>
       </c>
-      <c r="O12" s="20">
+      <c r="O12" s="22">
         <v>181</v>
       </c>
-      <c r="P12" s="20">
+      <c r="P12" s="22">
         <v>182</v>
       </c>
       <c r="Q12" s="19">

</xml_diff>